<commit_message>
mudança no banco de dados
</commit_message>
<xml_diff>
--- a/Documentacao/BackLog de Requisitos - ChessCode.xlsx
+++ b/Documentacao/BackLog de Requisitos - ChessCode.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateu\ChessCode\Documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{66D94D7F-EB28-4886-9F7A-182AA44CC044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36DC072F-9F4E-4AE8-A91C-9D357D8F0D4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9156" yWindow="0" windowWidth="13980" windowHeight="12336" xr2:uid="{240B8422-38C4-410A-92FD-61370D50BED2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{240B8422-38C4-410A-92FD-61370D50BED2}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="110">
   <si>
     <t>SPRINT</t>
   </si>
@@ -191,12 +191,6 @@
     <t>Página que terá todos os campeões da copa do mundo de xadrez organizado pela FIDE</t>
   </si>
   <si>
-    <t>Tela de figuras históricas do xadrez</t>
-  </si>
-  <si>
-    <t>Página que terá as maiores figuras históricas mundias da atualidade e do passado, globais e nacionais.</t>
-  </si>
-  <si>
     <t>Tela de Dashboard para os administradores</t>
   </si>
   <si>
@@ -363,6 +357,15 @@
   </si>
   <si>
     <t>MÉDIA</t>
+  </si>
+  <si>
+    <t>Tela sobre o xadrea</t>
+  </si>
+  <si>
+    <t>Página que terá informações sobre o xadrez, o formato do tabuleiro e sobre as peças de xadrez.</t>
+  </si>
+  <si>
+    <t>Sprint1</t>
   </si>
 </sst>
 </file>
@@ -636,17 +639,23 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -658,19 +667,13 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1016,20 +1019,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDC8D886-CB9B-4AED-8453-F33DBF6EA1ED}">
   <dimension ref="D3:AC34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="57" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="45" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="3" width="8.88671875" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="53.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="99.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.21875" customWidth="1"/>
+    <col min="6" max="6" width="64.88671875" customWidth="1"/>
     <col min="7" max="7" width="21.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" customWidth="1"/>
+    <col min="9" max="9" width="9.109375" customWidth="1"/>
+    <col min="10" max="10" width="6.5546875" customWidth="1"/>
     <col min="11" max="11" width="14.44140625" customWidth="1"/>
     <col min="14" max="14" width="12" customWidth="1"/>
     <col min="15" max="15" width="15.5546875" customWidth="1"/>
@@ -1044,30 +1047,30 @@
   </cols>
   <sheetData>
     <row r="3" spans="4:29" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="N3" s="17" t="s">
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="N3" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14"/>
-      <c r="V3" s="10"/>
-      <c r="W3" s="10"/>
-      <c r="X3" s="10"/>
-      <c r="Y3" s="10"/>
-      <c r="Z3" s="10"/>
-      <c r="AA3" s="10"/>
-      <c r="AB3" s="10"/>
-      <c r="AC3" s="10"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+      <c r="V3" s="14"/>
+      <c r="W3" s="14"/>
+      <c r="X3" s="14"/>
+      <c r="Y3" s="14"/>
+      <c r="Z3" s="14"/>
+      <c r="AA3" s="14"/>
+      <c r="AB3" s="14"/>
+      <c r="AC3" s="14"/>
     </row>
     <row r="4" spans="4:29" ht="21" x14ac:dyDescent="0.4">
       <c r="D4" s="1" t="s">
@@ -1094,55 +1097,55 @@
       <c r="K4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="N4" s="19" t="s">
+      <c r="N4" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="O4" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="P4" s="19" t="s">
+      <c r="O4" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="P4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="Q4" s="19" t="s">
+      <c r="Q4" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="4:29" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="N5" s="20">
-        <v>1</v>
-      </c>
-      <c r="O5" s="21">
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="N5" s="11">
+        <v>1</v>
+      </c>
+      <c r="O5" s="12">
         <v>45774</v>
       </c>
-      <c r="P5" s="21">
+      <c r="P5" s="12">
         <v>45781</v>
       </c>
-      <c r="Q5" s="20">
+      <c r="Q5" s="11">
         <f>SUM(I26+I27+I28+I29+I30+I31+I32+I33+I34)</f>
         <v>48</v>
       </c>
-      <c r="T5" s="10"/>
-      <c r="U5" s="10"/>
-      <c r="V5" s="10"/>
-      <c r="W5" s="10"/>
-      <c r="X5" s="10"/>
-      <c r="Y5" s="10"/>
-      <c r="Z5" s="10"/>
-      <c r="AA5" s="10"/>
+      <c r="T5" s="14"/>
+      <c r="U5" s="14"/>
+      <c r="V5" s="14"/>
+      <c r="W5" s="14"/>
+      <c r="X5" s="14"/>
+      <c r="Y5" s="14"/>
+      <c r="Z5" s="14"/>
+      <c r="AA5" s="14"/>
     </row>
     <row r="6" spans="4:29" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D6" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>23</v>
@@ -1165,23 +1168,23 @@
       <c r="K6" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="N6" s="20">
+      <c r="N6" s="11">
         <v>2</v>
       </c>
-      <c r="O6" s="21">
+      <c r="O6" s="12">
         <v>45782</v>
       </c>
-      <c r="P6" s="21">
+      <c r="P6" s="12">
         <v>45789</v>
       </c>
-      <c r="Q6" s="20">
+      <c r="Q6" s="11">
         <f>SUM(I6+I7+I8+I9+I10+I11+I12+I19)</f>
         <v>43</v>
       </c>
     </row>
     <row r="7" spans="4:29" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D7" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>24</v>
@@ -1204,23 +1207,23 @@
       <c r="K7" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="N7" s="20">
+      <c r="N7" s="11">
         <v>3</v>
       </c>
-      <c r="O7" s="21">
+      <c r="O7" s="12">
         <v>45790</v>
       </c>
-      <c r="P7" s="21">
+      <c r="P7" s="12">
         <v>45797</v>
       </c>
-      <c r="Q7" s="20">
+      <c r="Q7" s="11">
         <f>SUM(I13+I21+I22+I23+I24+I25)</f>
         <v>53</v>
       </c>
     </row>
     <row r="8" spans="4:29" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D8" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>25</v>
@@ -1243,23 +1246,23 @@
       <c r="K8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="N8" s="20">
+      <c r="N8" s="11">
         <v>4</v>
       </c>
-      <c r="O8" s="21">
+      <c r="O8" s="12">
         <v>45798</v>
       </c>
-      <c r="P8" s="21">
+      <c r="P8" s="12">
         <v>45805</v>
       </c>
-      <c r="Q8" s="20">
+      <c r="Q8" s="11">
         <f>SUM(I14+I15+I16+I17+I18)</f>
         <v>50</v>
       </c>
     </row>
     <row r="9" spans="4:29" ht="73.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D9" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>49</v>
@@ -1282,25 +1285,25 @@
       <c r="K9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="N9" s="18" t="s">
+      <c r="N9" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="O9" s="15"/>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="22">
+      <c r="O9" s="17"/>
+      <c r="P9" s="18"/>
+      <c r="Q9" s="13">
         <f>SUM(Q5+Q6+Q7+Q8)</f>
         <v>194</v>
       </c>
     </row>
     <row r="10" spans="4:29" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D10" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>51</v>
+        <v>107</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>52</v>
+        <v>108</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>17</v>
@@ -1317,19 +1320,19 @@
       <c r="K10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="N10" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="O10" s="15"/>
-      <c r="P10" s="16"/>
-      <c r="Q10" s="22">
+      <c r="N10" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="O10" s="17"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="13">
         <f>AVERAGE(AVERAGE(Q9)/4)</f>
         <v>48.5</v>
       </c>
     </row>
     <row r="11" spans="4:29" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D11" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>26</v>
@@ -1355,7 +1358,7 @@
     </row>
     <row r="12" spans="4:29" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D12" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>27</v>
@@ -1381,7 +1384,7 @@
     </row>
     <row r="13" spans="4:29" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D13" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>28</v>
@@ -1407,13 +1410,13 @@
     </row>
     <row r="14" spans="4:29" ht="73.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D14" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>17</v>
@@ -1433,13 +1436,13 @@
     </row>
     <row r="15" spans="4:29" ht="21" x14ac:dyDescent="0.3">
       <c r="D15" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>17</v>
@@ -1459,10 +1462,10 @@
     </row>
     <row r="16" spans="4:29" ht="63" x14ac:dyDescent="0.3">
       <c r="D16" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>47</v>
@@ -1482,18 +1485,18 @@
       <c r="K16" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="V16" s="10"/>
-      <c r="W16" s="10"/>
-      <c r="X16" s="10"/>
-      <c r="Y16" s="10"/>
-      <c r="Z16" s="10"/>
-      <c r="AA16" s="10"/>
-      <c r="AB16" s="10"/>
-      <c r="AC16" s="10"/>
+      <c r="V16" s="14"/>
+      <c r="W16" s="14"/>
+      <c r="X16" s="14"/>
+      <c r="Y16" s="14"/>
+      <c r="Z16" s="14"/>
+      <c r="AA16" s="14"/>
+      <c r="AB16" s="14"/>
+      <c r="AC16" s="14"/>
     </row>
     <row r="17" spans="4:11" ht="42" x14ac:dyDescent="0.3">
       <c r="D17" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>15</v>
@@ -1519,13 +1522,13 @@
     </row>
     <row r="18" spans="4:11" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D18" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>18</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>3</v>
@@ -1545,13 +1548,13 @@
     </row>
     <row r="19" spans="4:11" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D19" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>3</v>
@@ -1570,20 +1573,20 @@
       </c>
     </row>
     <row r="20" spans="4:11" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
     </row>
     <row r="21" spans="4:11" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D21" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>29</v>
@@ -1609,13 +1612,13 @@
     </row>
     <row r="22" spans="4:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D22" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G22" s="6" t="s">
         <v>3</v>
@@ -1635,13 +1638,13 @@
     </row>
     <row r="23" spans="4:11" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D23" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>3</v>
@@ -1661,13 +1664,13 @@
     </row>
     <row r="24" spans="4:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D24" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>30</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>3</v>
@@ -1687,13 +1690,13 @@
     </row>
     <row r="25" spans="4:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D25" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>31</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>3</v>
@@ -1713,7 +1716,7 @@
     </row>
     <row r="26" spans="4:11" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D26" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>35</v>
@@ -1739,7 +1742,7 @@
     </row>
     <row r="27" spans="4:11" ht="21" x14ac:dyDescent="0.3">
       <c r="D27" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>32</v>
@@ -1765,13 +1768,13 @@
     </row>
     <row r="28" spans="4:11" ht="21" x14ac:dyDescent="0.3">
       <c r="D28" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>17</v>
@@ -1791,13 +1794,13 @@
     </row>
     <row r="29" spans="4:11" ht="21" x14ac:dyDescent="0.3">
       <c r="D29" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>17</v>
@@ -1817,13 +1820,13 @@
     </row>
     <row r="30" spans="4:11" ht="21" x14ac:dyDescent="0.3">
       <c r="D30" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>17</v>
@@ -1843,13 +1846,13 @@
     </row>
     <row r="31" spans="4:11" ht="21" x14ac:dyDescent="0.3">
       <c r="D31" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>17</v>
@@ -1869,13 +1872,13 @@
     </row>
     <row r="32" spans="4:11" ht="21" x14ac:dyDescent="0.3">
       <c r="D32" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>17</v>
@@ -1895,13 +1898,13 @@
     </row>
     <row r="33" spans="4:11" ht="21" x14ac:dyDescent="0.3">
       <c r="D33" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>17</v>
@@ -1921,13 +1924,13 @@
     </row>
     <row r="34" spans="4:11" ht="21" x14ac:dyDescent="0.3">
       <c r="D34" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>17</v>
@@ -1942,7 +1945,7 @@
         <v>1</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>5</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1963,6 +1966,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010045B33021656A9E479DF12B9A8EE42828" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5ede22190f62034867da76e552493950">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="1dc861b8-2196-455d-b291-a999da8cffb6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7b92c7a709487a617ea736db7e12b693" ns3:_="">
     <xsd:import namespace="1dc861b8-2196-455d-b291-a999da8cffb6"/>
@@ -2144,15 +2156,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2162,6 +2165,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{879ABC2B-24C8-42D6-A379-5D9E812A53A4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B1DD218-DDF4-49B7-912F-990F90DABBF3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2175,14 +2186,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{879ABC2B-24C8-42D6-A379-5D9E812A53A4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>